<commit_message>
Updated results and analysis - hard coded 8 in the OpenMP statement threw the analysis and results off a bit
</commit_message>
<xml_diff>
--- a/nbody/Results/Analysis.xlsx
+++ b/nbody/Results/Analysis.xlsx
@@ -1852,7 +1852,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C70F-4768-9377-E46470A04882}"/>
@@ -1922,30 +1922,30 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>148</c:v>
+                  <c:v>405</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>545</c:v>
+                  <c:v>1614</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2115</c:v>
+                  <c:v>6469</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8767</c:v>
+                  <c:v>25910</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-C70F-4768-9377-E46470A04882}"/>
@@ -2015,30 +2015,30 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>47</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>149</c:v>
+                  <c:v>211</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>543</c:v>
+                  <c:v>835</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2137</c:v>
+                  <c:v>3376</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8445</c:v>
+                  <c:v>14009</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-C70F-4768-9377-E46470A04882}"/>
@@ -2108,30 +2108,30 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>148</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>546</c:v>
+                  <c:v>542</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2119</c:v>
+                  <c:v>2175</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8352</c:v>
+                  <c:v>8652</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-C70F-4768-9377-E46470A04882}"/>
@@ -2585,30 +2585,30 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.625</c:v>
+                  <c:v>2.1666666666666665</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9090909090909092</c:v>
+                  <c:v>2.0769230769230771</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.6956521739130439</c:v>
+                  <c:v>2.1386138613861387</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8445945945945947</c:v>
+                  <c:v>2.1358024691358026</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.3614678899082566</c:v>
+                  <c:v>2.148079306071871</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.5361702127659571</c:v>
+                  <c:v>2.136960890400371</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.2978213756130943</c:v>
+                  <c:v>2.1309532998842147</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-35D2-4B2B-8226-BA71B2FA3435}"/>
@@ -2678,30 +2678,30 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2.6</c:v>
+                  <c:v>4.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3.8571428571428572</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.5957446808510642</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8053691275167782</c:v>
+                  <c:v>4.0995260663507107</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.3848987108655617</c:v>
+                  <c:v>4.1520958083832333</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.4688816097332706</c:v>
+                  <c:v>4.0947867298578196</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.5379514505624634</c:v>
+                  <c:v>3.9412520522521235</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-35D2-4B2B-8226-BA71B2FA3435}"/>
@@ -2771,30 +2771,30 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2.1666666666666665</c:v>
+                  <c:v>3.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9090909090909092</c:v>
+                  <c:v>5.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.6956521739130439</c:v>
+                  <c:v>5.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8445945945945947</c:v>
+                  <c:v>6.1785714285714288</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.3498168498168495</c:v>
+                  <c:v>6.3966789667896675</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.5238319962246338</c:v>
+                  <c:v>6.355862068965517</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.6107519157088124</c:v>
+                  <c:v>6.3815302820157189</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-35D2-4B2B-8226-BA71B2FA3435}"/>
@@ -3249,30 +3249,30 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.8125</c:v>
+                  <c:v>1.0833333333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4545454545454546</c:v>
+                  <c:v>1.0384615384615385</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.347826086956522</c:v>
+                  <c:v>1.0693069306930694</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.9222972972972974</c:v>
+                  <c:v>1.0679012345679013</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.1807339449541283</c:v>
+                  <c:v>1.0740396530359355</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.2680851063829786</c:v>
+                  <c:v>1.0684804452001855</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.1489106878065471</c:v>
+                  <c:v>1.0654766499421073</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7C32-45D9-92E7-7ED55AC7E04C}"/>
@@ -3342,30 +3342,30 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.65</c:v>
+                  <c:v>1.0833333333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.9642857142857143</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1489361702127661</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4513422818791946</c:v>
+                  <c:v>1.0248815165876777</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5962246777163904</c:v>
+                  <c:v>1.0380239520958083</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6172204024333177</c:v>
+                  <c:v>1.0236966824644549</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6344878626406159</c:v>
+                  <c:v>0.98531301306303087</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7C32-45D9-92E7-7ED55AC7E04C}"/>
@@ -3435,30 +3435,30 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.27083333333333331</c:v>
+                  <c:v>0.40625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.61363636363636365</c:v>
+                  <c:v>0.67500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.58695652173913049</c:v>
+                  <c:v>0.67500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.73057432432432434</c:v>
+                  <c:v>0.7723214285714286</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.79372710622710618</c:v>
+                  <c:v>0.79958487084870844</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.81547899952807923</c:v>
+                  <c:v>0.79448275862068962</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.82634398946360155</c:v>
+                  <c:v>0.79769128525196487</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-7C32-45D9-92E7-7ED55AC7E04C}"/>
@@ -6046,8 +6046,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5696790" y="1409700"/>
-          <a:ext cx="7699282" cy="4741170"/>
+          <a:off x="5677580" y="1409700"/>
+          <a:ext cx="7656059" cy="4762781"/>
           <a:chOff x="5696790" y="1409700"/>
           <a:chExt cx="7699282" cy="4741170"/>
         </a:xfrm>
@@ -6185,8 +6185,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="20764500" y="3766297"/>
-          <a:ext cx="4572000" cy="2743200"/>
+          <a:off x="20654842" y="3783106"/>
+          <a:ext cx="4550389" cy="2748002"/>
           <a:chOff x="20764500" y="3766297"/>
           <a:chExt cx="4572000" cy="2743200"/>
         </a:xfrm>
@@ -6213,7 +6213,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="21829059" y="6185647"/>
+            <a:off x="21829059" y="6185646"/>
             <a:ext cx="713400" cy="264560"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -6277,7 +6277,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15867529" y="6164356"/>
+          <a:off x="15789889" y="6185967"/>
           <a:ext cx="713400" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6663,8 +6663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BQ46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7212,43 +7212,43 @@
         <v>55213</v>
       </c>
       <c r="D7">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="E7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F7">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="G7">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="H7">
-        <v>8767</v>
+        <v>25910</v>
       </c>
       <c r="I7">
-        <v>2137</v>
+        <v>3376</v>
       </c>
       <c r="J7">
         <v>13</v>
       </c>
       <c r="K7">
-        <v>2119</v>
+        <v>2175</v>
       </c>
       <c r="L7">
-        <v>543</v>
+        <v>835</v>
       </c>
       <c r="M7">
-        <v>8352</v>
+        <v>8652</v>
       </c>
       <c r="N7">
-        <v>46</v>
+        <v>101</v>
       </c>
       <c r="O7">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="P7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="Q7">
         <v>14</v>
@@ -7257,13 +7257,13 @@
         <v>13824</v>
       </c>
       <c r="S7">
-        <v>545</v>
+        <v>1614</v>
       </c>
       <c r="T7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="U7">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="V7">
         <v>3467</v>
@@ -7275,19 +7275,19 @@
         <v>865</v>
       </c>
       <c r="Y7">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z7">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="AA7">
-        <v>8445</v>
+        <v>14009</v>
       </c>
       <c r="AB7">
-        <v>148</v>
+        <v>405</v>
       </c>
       <c r="AC7">
-        <v>2115</v>
+        <v>6469</v>
       </c>
     </row>
     <row r="10" spans="1:69" x14ac:dyDescent="0.25">
@@ -7359,30 +7359,30 @@
       </c>
       <c r="N13" s="6">
         <f t="shared" ref="N13:N19" si="0">$B14/C14</f>
-        <v>1.625</v>
+        <v>2.1666666666666665</v>
       </c>
       <c r="O13" s="6">
         <f t="shared" ref="O13:P13" si="1">$B14/D14</f>
-        <v>2.6</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="P13" s="7">
         <f t="shared" si="1"/>
-        <v>2.1666666666666665</v>
+        <v>3.25</v>
       </c>
       <c r="R13" s="14">
         <v>512</v>
       </c>
       <c r="S13" s="4">
         <f>N13/S$12</f>
-        <v>0.8125</v>
+        <v>1.0833333333333333</v>
       </c>
       <c r="T13" s="4">
         <f>O13/T$12</f>
-        <v>0.65</v>
+        <v>1.0833333333333333</v>
       </c>
       <c r="U13" s="5">
         <f t="shared" ref="U13" si="2">P13/U$12</f>
-        <v>0.27083333333333331</v>
+        <v>0.40625</v>
       </c>
     </row>
     <row r="14" spans="1:69" ht="15.75" x14ac:dyDescent="0.25">
@@ -7393,13 +7393,13 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E14">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M14" s="14">
         <f>M13*2</f>
@@ -7407,7 +7407,7 @@
       </c>
       <c r="N14" s="6">
         <f t="shared" si="0"/>
-        <v>4.9090909090909092</v>
+        <v>2.0769230769230771</v>
       </c>
       <c r="O14" s="6">
         <f>$B15/D15</f>
@@ -7415,7 +7415,7 @@
       </c>
       <c r="P14" s="7">
         <f>$B15/E15</f>
-        <v>4.9090909090909092</v>
+        <v>5.4</v>
       </c>
       <c r="R14" s="14">
         <f>R13*2</f>
@@ -7423,7 +7423,7 @@
       </c>
       <c r="S14" s="4">
         <f>N14/S$12</f>
-        <v>2.4545454545454546</v>
+        <v>1.0384615384615385</v>
       </c>
       <c r="T14" s="4">
         <f>O14/T$12</f>
@@ -7431,7 +7431,7 @@
       </c>
       <c r="U14" s="5">
         <f>P14/U$12</f>
-        <v>0.61363636363636365</v>
+        <v>0.67500000000000004</v>
       </c>
     </row>
     <row r="15" spans="1:69" ht="15.75" x14ac:dyDescent="0.25">
@@ -7442,13 +7442,13 @@
         <v>54</v>
       </c>
       <c r="C15">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D15">
         <v>14</v>
       </c>
       <c r="E15">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M15" s="14">
         <f t="shared" ref="M15:M19" si="3">M14*2</f>
@@ -7456,15 +7456,15 @@
       </c>
       <c r="N15" s="6">
         <f t="shared" si="0"/>
-        <v>4.6956521739130439</v>
+        <v>2.1386138613861387</v>
       </c>
       <c r="O15" s="6">
         <f>$B16/D16</f>
-        <v>4.5957446808510642</v>
+        <v>4</v>
       </c>
       <c r="P15" s="7">
         <f t="shared" ref="P15:P19" si="4">$B16/E16</f>
-        <v>4.6956521739130439</v>
+        <v>5.4</v>
       </c>
       <c r="R15" s="14">
         <f t="shared" ref="R15:R19" si="5">R14*2</f>
@@ -7472,15 +7472,15 @@
       </c>
       <c r="S15" s="4">
         <f t="shared" ref="S15:S19" si="6">N15/S$12</f>
-        <v>2.347826086956522</v>
+        <v>1.0693069306930694</v>
       </c>
       <c r="T15" s="4">
         <f t="shared" ref="T15:T19" si="7">O15/T$12</f>
-        <v>1.1489361702127661</v>
+        <v>1</v>
       </c>
       <c r="U15" s="5">
         <f t="shared" ref="U15:U19" si="8">P15/U$12</f>
-        <v>0.58695652173913049</v>
+        <v>0.67500000000000004</v>
       </c>
     </row>
     <row r="16" spans="1:69" ht="15.75" x14ac:dyDescent="0.25">
@@ -7491,13 +7491,13 @@
         <v>216</v>
       </c>
       <c r="C16">
-        <v>46</v>
+        <v>101</v>
       </c>
       <c r="D16">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E16">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="M16" s="14">
         <f t="shared" si="3"/>
@@ -7505,15 +7505,15 @@
       </c>
       <c r="N16" s="6">
         <f t="shared" si="0"/>
-        <v>5.8445945945945947</v>
+        <v>2.1358024691358026</v>
       </c>
       <c r="O16" s="6">
         <f>$B17/D17</f>
-        <v>5.8053691275167782</v>
+        <v>4.0995260663507107</v>
       </c>
       <c r="P16" s="7">
         <f t="shared" si="4"/>
-        <v>5.8445945945945947</v>
+        <v>6.1785714285714288</v>
       </c>
       <c r="R16" s="14">
         <f t="shared" si="5"/>
@@ -7521,15 +7521,15 @@
       </c>
       <c r="S16" s="4">
         <f t="shared" si="6"/>
-        <v>2.9222972972972974</v>
+        <v>1.0679012345679013</v>
       </c>
       <c r="T16" s="4">
         <f t="shared" si="7"/>
-        <v>1.4513422818791946</v>
+        <v>1.0248815165876777</v>
       </c>
       <c r="U16" s="5">
         <f t="shared" si="8"/>
-        <v>0.73057432432432434</v>
+        <v>0.7723214285714286</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -7540,13 +7540,13 @@
         <v>865</v>
       </c>
       <c r="C17">
-        <v>148</v>
+        <v>405</v>
       </c>
       <c r="D17">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="E17">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="M17" s="14">
         <f t="shared" si="3"/>
@@ -7554,15 +7554,15 @@
       </c>
       <c r="N17" s="6">
         <f t="shared" si="0"/>
-        <v>6.3614678899082566</v>
+        <v>2.148079306071871</v>
       </c>
       <c r="O17" s="6">
         <f>$B18/D18</f>
-        <v>6.3848987108655617</v>
+        <v>4.1520958083832333</v>
       </c>
       <c r="P17" s="7">
         <f t="shared" si="4"/>
-        <v>6.3498168498168495</v>
+        <v>6.3966789667896675</v>
       </c>
       <c r="R17" s="14">
         <f t="shared" si="5"/>
@@ -7570,15 +7570,15 @@
       </c>
       <c r="S17" s="4">
         <f t="shared" si="6"/>
-        <v>3.1807339449541283</v>
+        <v>1.0740396530359355</v>
       </c>
       <c r="T17" s="4">
         <f t="shared" si="7"/>
-        <v>1.5962246777163904</v>
+        <v>1.0380239520958083</v>
       </c>
       <c r="U17" s="5">
         <f t="shared" si="8"/>
-        <v>0.79372710622710618</v>
+        <v>0.79958487084870844</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -7589,13 +7589,13 @@
         <v>3467</v>
       </c>
       <c r="C18">
-        <v>545</v>
+        <v>1614</v>
       </c>
       <c r="D18">
-        <v>543</v>
+        <v>835</v>
       </c>
       <c r="E18">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="M18" s="14">
         <f t="shared" si="3"/>
@@ -7603,15 +7603,15 @@
       </c>
       <c r="N18" s="6">
         <f t="shared" si="0"/>
-        <v>6.5361702127659571</v>
+        <v>2.136960890400371</v>
       </c>
       <c r="O18" s="6">
         <f>$B19/D19</f>
-        <v>6.4688816097332706</v>
+        <v>4.0947867298578196</v>
       </c>
       <c r="P18" s="7">
         <f t="shared" si="4"/>
-        <v>6.5238319962246338</v>
+        <v>6.355862068965517</v>
       </c>
       <c r="R18" s="14">
         <f t="shared" si="5"/>
@@ -7619,15 +7619,15 @@
       </c>
       <c r="S18" s="4">
         <f t="shared" si="6"/>
-        <v>3.2680851063829786</v>
+        <v>1.0684804452001855</v>
       </c>
       <c r="T18" s="4">
         <f t="shared" si="7"/>
-        <v>1.6172204024333177</v>
+        <v>1.0236966824644549</v>
       </c>
       <c r="U18" s="5">
         <f t="shared" si="8"/>
-        <v>0.81547899952807923</v>
+        <v>0.79448275862068962</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -7638,13 +7638,13 @@
         <v>13824</v>
       </c>
       <c r="C19">
-        <v>2115</v>
+        <v>6469</v>
       </c>
       <c r="D19">
-        <v>2137</v>
+        <v>3376</v>
       </c>
       <c r="E19">
-        <v>2119</v>
+        <v>2175</v>
       </c>
       <c r="M19" s="15">
         <f t="shared" si="3"/>
@@ -7652,15 +7652,15 @@
       </c>
       <c r="N19" s="8">
         <f t="shared" si="0"/>
-        <v>6.2978213756130943</v>
+        <v>2.1309532998842147</v>
       </c>
       <c r="O19" s="8">
         <f>$B20/D20</f>
-        <v>6.5379514505624634</v>
+        <v>3.9412520522521235</v>
       </c>
       <c r="P19" s="9">
         <f t="shared" si="4"/>
-        <v>6.6107519157088124</v>
+        <v>6.3815302820157189</v>
       </c>
       <c r="R19" s="15">
         <f t="shared" si="5"/>
@@ -7668,15 +7668,15 @@
       </c>
       <c r="S19" s="10">
         <f t="shared" si="6"/>
-        <v>3.1489106878065471</v>
+        <v>1.0654766499421073</v>
       </c>
       <c r="T19" s="10">
         <f t="shared" si="7"/>
-        <v>1.6344878626406159</v>
+        <v>0.98531301306303087</v>
       </c>
       <c r="U19" s="11">
         <f t="shared" si="8"/>
-        <v>0.82634398946360155</v>
+        <v>0.79769128525196487</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -7687,13 +7687,13 @@
         <v>55213</v>
       </c>
       <c r="C20">
-        <v>8767</v>
+        <v>25910</v>
       </c>
       <c r="D20">
-        <v>8445</v>
+        <v>14009</v>
       </c>
       <c r="E20">
-        <v>8352</v>
+        <v>8652</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated results - efficiency was rounded too much, resulted in 0s
</commit_message>
<xml_diff>
--- a/nbody/Results/Analysis.xlsx
+++ b/nbody/Results/Analysis.xlsx
@@ -616,7 +616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -713,6 +713,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3973,7 +4000,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$78:$B$84</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>8.6666666666666661</c:v>
@@ -4066,7 +4093,7 @@
             <c:numRef>
               <c:f>Sheet1!$C$78:$C$84</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.54166666666666663</c:v>
@@ -4159,7 +4186,7 @@
             <c:numRef>
               <c:f>Sheet1!$D$78:$D$84</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.33854166666666669</c:v>
@@ -4252,7 +4279,7 @@
             <c:numRef>
               <c:f>Sheet1!$E$78:$E$84</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.13541666666666666</c:v>
@@ -4345,7 +4372,7 @@
             <c:numRef>
               <c:f>Sheet1!$F$78:$F$84</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>5.3453947368421052E-2</c:v>
@@ -4438,7 +4465,7 @@
             <c:numRef>
               <c:f>Sheet1!$G$78:$G$84</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>3.3854166666666664E-2</c:v>
@@ -4531,7 +4558,7 @@
             <c:numRef>
               <c:f>Sheet1!$H$78:$H$84</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.8136160714285716E-2</c:v>
@@ -4626,7 +4653,7 @@
             <c:numRef>
               <c:f>Sheet1!$I$78:$I$84</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2.5390625E-2</c:v>
@@ -4855,7 +4882,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -9795,15 +9822,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="delete_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="delete" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="delete" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="delete_2" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="delete_2" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="delete_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10071,8 +10098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BQ86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M147" sqref="M147"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78:I84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11934,35 +11961,35 @@
       <c r="A78" s="24">
         <v>512</v>
       </c>
-      <c r="B78" s="33">
+      <c r="B78" s="52">
         <f>B52/B$77</f>
         <v>8.6666666666666661</v>
       </c>
-      <c r="C78" s="34">
+      <c r="C78" s="53">
         <f>C52/C$77</f>
         <v>0.54166666666666663</v>
       </c>
-      <c r="D78" s="34">
+      <c r="D78" s="53">
         <f t="shared" ref="D78:I78" si="11">D52/D$77</f>
         <v>0.33854166666666669</v>
       </c>
-      <c r="E78" s="34">
+      <c r="E78" s="53">
         <f t="shared" si="11"/>
         <v>0.13541666666666666</v>
       </c>
-      <c r="F78" s="34">
+      <c r="F78" s="53">
         <f t="shared" si="11"/>
         <v>5.3453947368421052E-2</v>
       </c>
-      <c r="G78" s="34">
+      <c r="G78" s="53">
         <f t="shared" si="11"/>
         <v>3.3854166666666664E-2</v>
       </c>
-      <c r="H78" s="34">
+      <c r="H78" s="53">
         <f t="shared" si="11"/>
         <v>1.8136160714285716E-2</v>
       </c>
-      <c r="I78" s="35">
+      <c r="I78" s="54">
         <f t="shared" si="11"/>
         <v>2.5390625E-2</v>
       </c>
@@ -11971,35 +11998,35 @@
       <c r="A79" s="25">
         <v>1024</v>
       </c>
-      <c r="B79" s="36">
+      <c r="B79" s="55">
         <f t="shared" ref="B79:C84" si="12">B53/B$77</f>
         <v>16.875</v>
       </c>
-      <c r="C79" s="37">
+      <c r="C79" s="56">
         <f t="shared" si="12"/>
         <v>1.875</v>
       </c>
-      <c r="D79" s="37">
+      <c r="D79" s="56">
         <f t="shared" ref="D79:I79" si="13">D53/D$77</f>
         <v>0.88815789473684215</v>
       </c>
-      <c r="E79" s="37">
+      <c r="E79" s="56">
         <f t="shared" si="13"/>
         <v>0.44407894736842107</v>
       </c>
-      <c r="F79" s="37">
+      <c r="F79" s="56">
         <f t="shared" si="13"/>
         <v>0.22203947368421054</v>
       </c>
-      <c r="G79" s="37">
+      <c r="G79" s="56">
         <f t="shared" si="13"/>
         <v>0.1171875</v>
       </c>
-      <c r="H79" s="37">
+      <c r="H79" s="56">
         <f t="shared" si="13"/>
         <v>5.859375E-2</v>
       </c>
-      <c r="I79" s="38">
+      <c r="I79" s="57">
         <f t="shared" si="13"/>
         <v>2.511160714285714E-2</v>
       </c>
@@ -12008,35 +12035,35 @@
       <c r="A80" s="25">
         <v>2048</v>
       </c>
-      <c r="B80" s="36">
+      <c r="B80" s="55">
         <f t="shared" si="12"/>
         <v>23.736263736263737</v>
       </c>
-      <c r="C80" s="37">
+      <c r="C80" s="56">
         <f t="shared" si="12"/>
         <v>4.8214285714285721</v>
       </c>
-      <c r="D80" s="37">
+      <c r="D80" s="56">
         <f t="shared" ref="D80:I80" si="14">D54/D$77</f>
         <v>1.9852941176470589</v>
       </c>
-      <c r="E80" s="37">
+      <c r="E80" s="56">
         <f t="shared" si="14"/>
         <v>1.205357142857143</v>
       </c>
-      <c r="F80" s="37">
+      <c r="F80" s="56">
         <f t="shared" si="14"/>
         <v>0.5818965517241379</v>
       </c>
-      <c r="G80" s="37">
+      <c r="G80" s="56">
         <f t="shared" si="14"/>
         <v>0.29094827586206895</v>
       </c>
-      <c r="H80" s="37">
+      <c r="H80" s="56">
         <f t="shared" si="14"/>
         <v>0.14547413793103448</v>
       </c>
-      <c r="I80" s="38">
+      <c r="I80" s="57">
         <f t="shared" si="14"/>
         <v>6.3920454545454544E-2</v>
       </c>
@@ -12045,35 +12072,35 @@
       <c r="A81" s="25">
         <v>4096</v>
       </c>
-      <c r="B81" s="36">
+      <c r="B81" s="55">
         <f t="shared" si="12"/>
         <v>25.218658892128282</v>
       </c>
-      <c r="C81" s="37">
+      <c r="C81" s="56">
         <f t="shared" si="12"/>
         <v>11.033163265306122</v>
       </c>
-      <c r="D81" s="37">
+      <c r="D81" s="56">
         <f t="shared" ref="D81:I81" si="15">D55/D$77</f>
         <v>4.3598790322580641</v>
       </c>
-      <c r="E81" s="37">
+      <c r="E81" s="56">
         <f t="shared" si="15"/>
         <v>2.7582908163265305</v>
       </c>
-      <c r="F81" s="37">
+      <c r="F81" s="56">
         <f t="shared" si="15"/>
         <v>1.3515625</v>
       </c>
-      <c r="G81" s="37">
+      <c r="G81" s="56">
         <f t="shared" si="15"/>
         <v>0.68957270408163263</v>
       </c>
-      <c r="H81" s="37">
+      <c r="H81" s="56">
         <f t="shared" si="15"/>
         <v>0.33126531862745101</v>
       </c>
-      <c r="I81" s="38">
+      <c r="I81" s="57">
         <f t="shared" si="15"/>
         <v>0.14078776041666666</v>
       </c>
@@ -12082,35 +12109,35 @@
       <c r="A82" s="25">
         <v>8192</v>
       </c>
-      <c r="B82" s="36">
+      <c r="B82" s="55">
         <f t="shared" si="12"/>
         <v>25.796130952380953</v>
       </c>
-      <c r="C82" s="37">
+      <c r="C82" s="56">
         <f t="shared" si="12"/>
         <v>16.9287109375</v>
       </c>
-      <c r="D82" s="37">
+      <c r="D82" s="56">
         <f t="shared" ref="D82:I82" si="16">D56/D$77</f>
         <v>7.8509963768115938</v>
       </c>
-      <c r="E82" s="37">
+      <c r="E82" s="56">
         <f t="shared" si="16"/>
         <v>3.9832261029411766</v>
       </c>
-      <c r="F82" s="37">
+      <c r="F82" s="56">
         <f t="shared" si="16"/>
         <v>2.0996850775193798</v>
       </c>
-      <c r="G82" s="37">
+      <c r="G82" s="56">
         <f t="shared" si="16"/>
         <v>1.0417668269230769</v>
       </c>
-      <c r="H82" s="37">
+      <c r="H82" s="56">
         <f t="shared" si="16"/>
         <v>0.50913416353383456</v>
       </c>
-      <c r="I82" s="38">
+      <c r="I82" s="57">
         <f t="shared" si="16"/>
         <v>0.26659387303149606</v>
       </c>
@@ -12119,35 +12146,35 @@
       <c r="A83" s="25">
         <v>16384</v>
       </c>
-      <c r="B83" s="36">
+      <c r="B83" s="55">
         <f t="shared" si="12"/>
         <v>25.853749766224048</v>
       </c>
-      <c r="C83" s="37">
+      <c r="C83" s="56">
         <f t="shared" si="12"/>
         <v>18.227848101265824</v>
       </c>
-      <c r="D83" s="37">
+      <c r="D83" s="56">
         <f t="shared" ref="D83:I83" si="17">D57/D$77</f>
         <v>9.9082568807339442</v>
       </c>
-      <c r="E83" s="37">
+      <c r="E83" s="56">
         <f t="shared" si="17"/>
         <v>4.9655172413793105</v>
       </c>
-      <c r="F83" s="37">
+      <c r="F83" s="56">
         <f t="shared" si="17"/>
         <v>2.5653206650831355</v>
       </c>
-      <c r="G83" s="37">
+      <c r="G83" s="56">
         <f t="shared" si="17"/>
         <v>1.2949640287769784</v>
       </c>
-      <c r="H83" s="37">
+      <c r="H83" s="56">
         <f t="shared" si="17"/>
         <v>0.62355658198614328</v>
       </c>
-      <c r="I83" s="38">
+      <c r="I83" s="57">
         <f t="shared" si="17"/>
         <v>0.31542056074766356</v>
       </c>
@@ -12156,35 +12183,35 @@
       <c r="A84" s="26">
         <v>32768</v>
       </c>
-      <c r="B84" s="51">
+      <c r="B84" s="58">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="C84" s="40">
+      <c r="C84" s="59">
         <f t="shared" si="12"/>
         <v>18.582727517501347</v>
       </c>
-      <c r="D84" s="40">
+      <c r="D84" s="59">
         <f t="shared" ref="D84:I84" si="18">D58/D$77</f>
         <v>10.419119867149758</v>
       </c>
-      <c r="E84" s="40">
+      <c r="E84" s="59">
         <f t="shared" si="18"/>
         <v>5.4636043381887269</v>
       </c>
-      <c r="F84" s="40">
+      <c r="F84" s="59">
         <f t="shared" si="18"/>
         <v>2.733533349176172</v>
       </c>
-      <c r="G84" s="40">
+      <c r="G84" s="59">
         <f t="shared" si="18"/>
         <v>1.3676333623969563</v>
       </c>
-      <c r="H84" s="40">
+      <c r="H84" s="59">
         <f t="shared" si="18"/>
         <v>0.68208659471853261</v>
       </c>
-      <c r="I84" s="41">
+      <c r="I84" s="60">
         <f t="shared" si="18"/>
         <v>0.34365165909815165</v>
       </c>

</xml_diff>